<commit_message>
Estilizando a página de inicio
</commit_message>
<xml_diff>
--- a/extras_files/cronograma_funcionalidades.xlsx
+++ b/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE6ECC6-3A17-4F9F-883F-BC52384270C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269D5C8C-31E4-419A-82DF-36AC186E0711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>FUNCIONALIDADE</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Uma página inicial que conterá(em um único HTML) informações sobre a pastoral, e sobre o Santuário também, nela não precisará estar logado para acessar, ou seja, ela é o intermedio entre as páginas necessárias para login e as não necessárias.</t>
+  </si>
+  <si>
+    <t>Relatar bugs</t>
+  </si>
+  <si>
+    <t>Um botão que ficará no dropdown do menu do usuário, e ao clicar nele, será redirecionado a um forms do google que permitirá a enviar ou relatar algum bug encontrado no sistema</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -215,9 +221,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -500,15 +503,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F16"/>
+  <dimension ref="B1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="36.5546875" customWidth="1"/>
+    <col min="2" max="4" width="36.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" customWidth="1"/>
     <col min="7" max="7" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -679,78 +684,93 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+    <row r="12" spans="2:6" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="6" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
+    <row r="15" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="6" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
+    <row r="16" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="6" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
+    <row r="17" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="6" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="3" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reformulei o campo grupo e criei uma tabela só para Grupos
</commit_message>
<xml_diff>
--- a/extras_files/cronograma_funcionalidades.xlsx
+++ b/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40225DC8-7083-4A4E-8784-AADDA4493436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6ADB67-43A5-44B8-8DA4-200FBD9BAD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
   <si>
     <t>FUNCIONALIDADE</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>NÃO FEITO</t>
+  </si>
+  <si>
+    <t>Parabenização na data de aniversário</t>
+  </si>
+  <si>
+    <t>Criar um sistema para que, quando o catequista logar no sistema, e sua data de aniversário for no dia ou tiver passado pelo menos 5 dias de sua data de aniversário, apareça um pop-up desejando felicitações pela sua data de nascimento</t>
   </si>
 </sst>
 </file>
@@ -259,11 +265,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -277,116 +283,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -664,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F18"/>
+  <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,15 +866,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>46</v>
@@ -984,16 +883,33 @@
         <v>29</v>
       </c>
     </row>
+    <row r="19" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E18">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",E2)))</formula>
+  <conditionalFormatting sqref="E2:E19">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NÃO FEITO">
+      <formula>NOT(ISERROR(SEARCH("NÃO FEITO",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FAZENDO">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAZENDO">
       <formula>NOT(ISERROR(SEARCH("FAZENDO",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NÃO FEITO">
-      <formula>NOT(ISERROR(SEARCH("NÃO FEITO",E2)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>